<commit_message>
changed dates to 2025 in DB
</commit_message>
<xml_diff>
--- a/project_db.xlsx
+++ b/project_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python projects\cdss\mini-project-cdss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\יונתן\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9DE236-21F6-4F76-9E3D-5DE62CDBDD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C1AD68-8011-4522-A988-3ED7B6C2AB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="54">
   <si>
     <t>First name</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>Katz</t>
-  </si>
-  <si>
-    <t>130</t>
   </si>
 </sst>
 </file>
@@ -553,14 +550,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="F271" sqref="F271"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="G322" sqref="G322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="31.375" customWidth="1"/>
-    <col min="7" max="7" width="40.125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
+    <col min="7" max="7" width="31.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -603,10 +601,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="2">
-        <v>43237.549305555563</v>
+        <v>45764.549305555563</v>
       </c>
       <c r="G2" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -626,10 +624,10 @@
         <v>10</v>
       </c>
       <c r="F3" s="2">
-        <v>43237.549305555563</v>
+        <v>45764.549305555563</v>
       </c>
       <c r="G3" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -649,10 +647,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="2">
-        <v>43238.625</v>
+        <v>45765.625</v>
       </c>
       <c r="G4" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -672,10 +670,10 @@
         <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>43237.708333333343</v>
+        <v>45764.708333333343</v>
       </c>
       <c r="G5" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -695,10 +693,10 @@
         <v>10</v>
       </c>
       <c r="F6" s="2">
-        <v>43238.458333333343</v>
+        <v>45765.458333333343</v>
       </c>
       <c r="G6" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -718,10 +716,10 @@
         <v>10</v>
       </c>
       <c r="F7" s="2">
-        <v>43238.541666666657</v>
+        <v>45765.541666666657</v>
       </c>
       <c r="G7" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -741,10 +739,10 @@
         <v>10</v>
       </c>
       <c r="F8" s="2">
-        <v>43238.791666666657</v>
+        <v>45765.791666666657</v>
       </c>
       <c r="G8" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -764,10 +762,10 @@
         <v>10</v>
       </c>
       <c r="F9" s="2">
-        <v>43239.127083333333</v>
+        <v>45766.127083333333</v>
       </c>
       <c r="G9" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -787,10 +785,10 @@
         <v>10</v>
       </c>
       <c r="F10" s="2">
-        <v>43240.458333333343</v>
+        <v>45767.458333333343</v>
       </c>
       <c r="G10" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -810,10 +808,10 @@
         <v>10</v>
       </c>
       <c r="F11" s="2">
-        <v>43241.291666666657</v>
+        <v>45768.291666666657</v>
       </c>
       <c r="G11" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -833,10 +831,10 @@
         <v>16</v>
       </c>
       <c r="F12" s="2">
-        <v>43239.115277777782</v>
+        <v>45766.115277777782</v>
       </c>
       <c r="G12" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -856,10 +854,10 @@
         <v>16</v>
       </c>
       <c r="F13" s="2">
-        <v>43240.089583333327</v>
+        <v>45767.089583333327</v>
       </c>
       <c r="G13" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -879,10 +877,10 @@
         <v>16</v>
       </c>
       <c r="F14" s="2">
-        <v>43241.113194444442</v>
+        <v>45768.113194444442</v>
       </c>
       <c r="G14" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -902,10 +900,10 @@
         <v>16</v>
       </c>
       <c r="F15" s="2">
-        <v>43239.115277777782</v>
+        <v>45766.115277777782</v>
       </c>
       <c r="G15" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -925,10 +923,10 @@
         <v>16</v>
       </c>
       <c r="F16" s="2">
-        <v>43240.089583333327</v>
+        <v>45767.089583333327</v>
       </c>
       <c r="G16" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -948,10 +946,10 @@
         <v>16</v>
       </c>
       <c r="F17" s="2">
-        <v>43241.113194444442</v>
+        <v>45768.113194444442</v>
       </c>
       <c r="G17" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -971,10 +969,10 @@
         <v>18</v>
       </c>
       <c r="F18" s="2">
-        <v>43237.414583333331</v>
+        <v>45764.414583333331</v>
       </c>
       <c r="G18" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -994,10 +992,10 @@
         <v>18</v>
       </c>
       <c r="F19" s="2">
-        <v>43237.444444444453</v>
+        <v>45764.444444444453</v>
       </c>
       <c r="G19" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1017,10 +1015,10 @@
         <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>43237.486805555563</v>
+        <v>45764.486805555563</v>
       </c>
       <c r="G20" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1040,10 +1038,10 @@
         <v>18</v>
       </c>
       <c r="F21" s="2">
-        <v>43237.549305555563</v>
+        <v>45764.549305555563</v>
       </c>
       <c r="G21" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1063,10 +1061,10 @@
         <v>18</v>
       </c>
       <c r="F22" s="2">
-        <v>43237.618750000001</v>
+        <v>45764.618750000001</v>
       </c>
       <c r="G22" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1086,10 +1084,10 @@
         <v>18</v>
       </c>
       <c r="F23" s="2">
-        <v>43237.666666666657</v>
+        <v>45764.666666666657</v>
       </c>
       <c r="G23" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1109,10 +1107,10 @@
         <v>18</v>
       </c>
       <c r="F24" s="2">
-        <v>43237.708333333343</v>
+        <v>45764.708333333343</v>
       </c>
       <c r="G24" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1132,10 +1130,10 @@
         <v>18</v>
       </c>
       <c r="F25" s="2">
-        <v>43237.75</v>
+        <v>45764.75</v>
       </c>
       <c r="G25" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1155,10 +1153,10 @@
         <v>18</v>
       </c>
       <c r="F26" s="2">
-        <v>43237.791666666657</v>
+        <v>45764.791666666657</v>
       </c>
       <c r="G26" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1178,10 +1176,10 @@
         <v>18</v>
       </c>
       <c r="F27" s="2">
-        <v>43237.833333333343</v>
+        <v>45764.833333333343</v>
       </c>
       <c r="G27" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1201,10 +1199,10 @@
         <v>18</v>
       </c>
       <c r="F28" s="2">
-        <v>43237.875</v>
+        <v>45764.875</v>
       </c>
       <c r="G28" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1224,10 +1222,10 @@
         <v>18</v>
       </c>
       <c r="F29" s="2">
-        <v>43237.875</v>
+        <v>45764.875</v>
       </c>
       <c r="G29" s="2">
-        <v>43243.583333333343</v>
+        <v>45770.583333333343</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1247,10 +1245,10 @@
         <v>18</v>
       </c>
       <c r="F30" s="2">
-        <v>43237.958333333343</v>
+        <v>45764.958333333343</v>
       </c>
       <c r="G30" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1270,10 +1268,10 @@
         <v>18</v>
       </c>
       <c r="F31" s="2">
-        <v>43238.041666666657</v>
+        <v>45765.041666666657</v>
       </c>
       <c r="G31" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1293,10 +1291,10 @@
         <v>18</v>
       </c>
       <c r="F32" s="2">
-        <v>43238.083333333343</v>
+        <v>45765.083333333343</v>
       </c>
       <c r="G32" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1316,10 +1314,10 @@
         <v>18</v>
       </c>
       <c r="F33" s="2">
-        <v>43238.125</v>
+        <v>45765.125</v>
       </c>
       <c r="G33" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1339,10 +1337,10 @@
         <v>18</v>
       </c>
       <c r="F34" s="2">
-        <v>43238.291666666657</v>
+        <v>45765.291666666657</v>
       </c>
       <c r="G34" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1362,10 +1360,10 @@
         <v>18</v>
       </c>
       <c r="F35" s="2">
-        <v>43238.458333333343</v>
+        <v>45765.458333333343</v>
       </c>
       <c r="G35" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1385,10 +1383,10 @@
         <v>18</v>
       </c>
       <c r="F36" s="2">
-        <v>43238.652083333327</v>
+        <v>45765.652083333327</v>
       </c>
       <c r="G36" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1408,10 +1406,10 @@
         <v>18</v>
       </c>
       <c r="F37" s="2">
-        <v>43239.127083333333</v>
+        <v>45766.127083333333</v>
       </c>
       <c r="G37" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1431,10 +1429,10 @@
         <v>18</v>
       </c>
       <c r="F38" s="2">
-        <v>43239.115277777782</v>
+        <v>45766.115277777782</v>
       </c>
       <c r="G38" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1454,10 +1452,10 @@
         <v>18</v>
       </c>
       <c r="F39" s="2">
-        <v>43239.456250000003</v>
+        <v>45766.456250000003</v>
       </c>
       <c r="G39" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1477,10 +1475,10 @@
         <v>18</v>
       </c>
       <c r="F40" s="2">
-        <v>43240.089583333327</v>
+        <v>45767.089583333327</v>
       </c>
       <c r="G40" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1500,10 +1498,10 @@
         <v>18</v>
       </c>
       <c r="F41" s="2">
-        <v>43240.458333333343</v>
+        <v>45767.458333333343</v>
       </c>
       <c r="G41" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1523,10 +1521,10 @@
         <v>18</v>
       </c>
       <c r="F42" s="2">
-        <v>43240.6875</v>
+        <v>45767.6875</v>
       </c>
       <c r="G42" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1546,10 +1544,10 @@
         <v>18</v>
       </c>
       <c r="F43" s="2">
-        <v>43240.916666666657</v>
+        <v>45767.916666666657</v>
       </c>
       <c r="G43" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1569,10 +1567,10 @@
         <v>18</v>
       </c>
       <c r="F44" s="2">
-        <v>43241.113194444442</v>
+        <v>45768.113194444442</v>
       </c>
       <c r="G44" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1592,10 +1590,10 @@
         <v>18</v>
       </c>
       <c r="F45" s="2">
-        <v>43237.604166666657</v>
+        <v>45764.604166666657</v>
       </c>
       <c r="G45" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1615,10 +1613,10 @@
         <v>18</v>
       </c>
       <c r="F46" s="2">
-        <v>43237.708333333343</v>
+        <v>45764.708333333343</v>
       </c>
       <c r="G46" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1638,10 +1636,10 @@
         <v>18</v>
       </c>
       <c r="F47" s="2">
-        <v>43237.791666666657</v>
+        <v>45764.791666666657</v>
       </c>
       <c r="G47" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1661,10 +1659,10 @@
         <v>18</v>
       </c>
       <c r="F48" s="2">
-        <v>43237.958333333343</v>
+        <v>45764.958333333343</v>
       </c>
       <c r="G48" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1684,10 +1682,10 @@
         <v>18</v>
       </c>
       <c r="F49" s="2">
-        <v>43238.125</v>
+        <v>45765.125</v>
       </c>
       <c r="G49" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1707,10 +1705,10 @@
         <v>18</v>
       </c>
       <c r="F50" s="2">
-        <v>43238.291666666657</v>
+        <v>45765.291666666657</v>
       </c>
       <c r="G50" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1730,10 +1728,10 @@
         <v>18</v>
       </c>
       <c r="F51" s="2">
-        <v>43238.458333333343</v>
+        <v>45765.458333333343</v>
       </c>
       <c r="G51" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1753,10 +1751,10 @@
         <v>18</v>
       </c>
       <c r="F52" s="2">
-        <v>43238.625</v>
+        <v>45765.625</v>
       </c>
       <c r="G52" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1776,10 +1774,10 @@
         <v>18</v>
       </c>
       <c r="F53" s="2">
-        <v>43239.083333333343</v>
+        <v>45766.083333333343</v>
       </c>
       <c r="G53" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1799,10 +1797,10 @@
         <v>18</v>
       </c>
       <c r="F54" s="2">
-        <v>43238.791666666657</v>
+        <v>45765.791666666657</v>
       </c>
       <c r="G54" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1822,10 +1820,10 @@
         <v>18</v>
       </c>
       <c r="F55" s="2">
-        <v>43239.291666666657</v>
+        <v>45766.291666666657</v>
       </c>
       <c r="G55" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1845,10 +1843,10 @@
         <v>18</v>
       </c>
       <c r="F56" s="2">
-        <v>43239.458333333343</v>
+        <v>45766.458333333343</v>
       </c>
       <c r="G56" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1868,10 +1866,10 @@
         <v>18</v>
       </c>
       <c r="F57" s="2">
-        <v>43240.291666666657</v>
+        <v>45767.291666666657</v>
       </c>
       <c r="G57" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -1891,10 +1889,10 @@
         <v>18</v>
       </c>
       <c r="F58" s="2">
-        <v>43240.458333333343</v>
+        <v>45767.458333333343</v>
       </c>
       <c r="G58" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -1914,10 +1912,10 @@
         <v>18</v>
       </c>
       <c r="F59" s="2">
-        <v>43241.291666666657</v>
+        <v>45768.291666666657</v>
       </c>
       <c r="G59" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1937,10 +1935,10 @@
         <v>18</v>
       </c>
       <c r="F60" s="2">
-        <v>43241.4375</v>
+        <v>45768.4375</v>
       </c>
       <c r="G60" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -1960,10 +1958,10 @@
         <v>18</v>
       </c>
       <c r="F61" s="2">
-        <v>43241.625</v>
+        <v>45768.625</v>
       </c>
       <c r="G61" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -1983,10 +1981,10 @@
         <v>26</v>
       </c>
       <c r="F62" s="2">
-        <v>43237.791666666657</v>
+        <v>45764.791666666657</v>
       </c>
       <c r="G62" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -2006,10 +2004,10 @@
         <v>26</v>
       </c>
       <c r="F63" s="2">
-        <v>43237.958333333343</v>
+        <v>45764.958333333343</v>
       </c>
       <c r="G63" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -2029,10 +2027,10 @@
         <v>26</v>
       </c>
       <c r="F64" s="2">
-        <v>43238.125</v>
+        <v>45765.125</v>
       </c>
       <c r="G64" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -2052,10 +2050,10 @@
         <v>26</v>
       </c>
       <c r="F65" s="2">
-        <v>43241.291666666657</v>
+        <v>45768.291666666657</v>
       </c>
       <c r="G65" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -2075,10 +2073,10 @@
         <v>26</v>
       </c>
       <c r="F66" s="2">
-        <v>43237.444444444453</v>
+        <v>45764.444444444453</v>
       </c>
       <c r="G66" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -2098,10 +2096,10 @@
         <v>26</v>
       </c>
       <c r="F67" s="2">
-        <v>43237.444444444453</v>
+        <v>45764.444444444453</v>
       </c>
       <c r="G67" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -2121,10 +2119,10 @@
         <v>26</v>
       </c>
       <c r="F68" s="2">
-        <v>43238.374305555553</v>
+        <v>45765.374305555553</v>
       </c>
       <c r="G68" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -2144,10 +2142,10 @@
         <v>26</v>
       </c>
       <c r="F69" s="2">
-        <v>43237.604166666657</v>
+        <v>45764.604166666657</v>
       </c>
       <c r="G69" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -2167,10 +2165,10 @@
         <v>26</v>
       </c>
       <c r="F70" s="2">
-        <v>43240.291666666657</v>
+        <v>45767.291666666657</v>
       </c>
       <c r="G70" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -2190,10 +2188,10 @@
         <v>26</v>
       </c>
       <c r="F71" s="2">
-        <v>43237.875</v>
+        <v>45764.875</v>
       </c>
       <c r="G71" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -2213,10 +2211,10 @@
         <v>26</v>
       </c>
       <c r="F72" s="2">
-        <v>43238.333333333343</v>
+        <v>45765.333333333343</v>
       </c>
       <c r="G72" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -2236,10 +2234,10 @@
         <v>28</v>
       </c>
       <c r="F73" s="2">
-        <v>43237.414583333331</v>
+        <v>45764.414583333331</v>
       </c>
       <c r="G73" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -2259,10 +2257,10 @@
         <v>28</v>
       </c>
       <c r="F74" s="2">
-        <v>43237.444444444453</v>
+        <v>45764.444444444453</v>
       </c>
       <c r="G74" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -2282,10 +2280,10 @@
         <v>28</v>
       </c>
       <c r="F75" s="2">
-        <v>43237.486805555563</v>
+        <v>45764.486805555563</v>
       </c>
       <c r="G75" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2305,10 +2303,10 @@
         <v>28</v>
       </c>
       <c r="F76" s="2">
-        <v>43237.549305555563</v>
+        <v>45764.549305555563</v>
       </c>
       <c r="G76" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2328,10 +2326,10 @@
         <v>28</v>
       </c>
       <c r="F77" s="2">
-        <v>43237.618750000001</v>
+        <v>45764.618750000001</v>
       </c>
       <c r="G77" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2351,10 +2349,10 @@
         <v>28</v>
       </c>
       <c r="F78" s="2">
-        <v>43237.821527777778</v>
+        <v>45764.821527777778</v>
       </c>
       <c r="G78" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2374,10 +2372,10 @@
         <v>28</v>
       </c>
       <c r="F79" s="2">
-        <v>43238.374305555553</v>
+        <v>45765.374305555553</v>
       </c>
       <c r="G79" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -2397,10 +2395,10 @@
         <v>28</v>
       </c>
       <c r="F80" s="2">
-        <v>43238.652083333327</v>
+        <v>45765.652083333327</v>
       </c>
       <c r="G80" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -2420,10 +2418,10 @@
         <v>28</v>
       </c>
       <c r="F81" s="2">
-        <v>43239.127083333333</v>
+        <v>45766.127083333333</v>
       </c>
       <c r="G81" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -2443,10 +2441,10 @@
         <v>28</v>
       </c>
       <c r="F82" s="2">
-        <v>43239.206250000003</v>
+        <v>45766.206250000003</v>
       </c>
       <c r="G82" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -2466,10 +2464,10 @@
         <v>28</v>
       </c>
       <c r="F83" s="2">
-        <v>43237.414583333331</v>
+        <v>45764.414583333331</v>
       </c>
       <c r="G83" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -2489,10 +2487,10 @@
         <v>28</v>
       </c>
       <c r="F84" s="2">
-        <v>43237.444444444453</v>
+        <v>45764.444444444453</v>
       </c>
       <c r="G84" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -2512,10 +2510,10 @@
         <v>28</v>
       </c>
       <c r="F85" s="2">
-        <v>43237.486805555563</v>
+        <v>45764.486805555563</v>
       </c>
       <c r="G85" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -2535,10 +2533,10 @@
         <v>28</v>
       </c>
       <c r="F86" s="2">
-        <v>43237.549305555563</v>
+        <v>45764.549305555563</v>
       </c>
       <c r="G86" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -2558,10 +2556,10 @@
         <v>28</v>
       </c>
       <c r="F87" s="2">
-        <v>43237.618750000001</v>
+        <v>45764.618750000001</v>
       </c>
       <c r="G87" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -2581,10 +2579,10 @@
         <v>28</v>
       </c>
       <c r="F88" s="2">
-        <v>43237.821527777778</v>
+        <v>45764.821527777778</v>
       </c>
       <c r="G88" s="2">
-        <v>43249.416666666657</v>
+        <v>45776.416666666657</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -2604,10 +2602,10 @@
         <v>28</v>
       </c>
       <c r="F89" s="2">
-        <v>43238.374305555553</v>
+        <v>45765.374305555553</v>
       </c>
       <c r="G89" s="2">
-        <v>43250.416666666657</v>
+        <v>45777.416666666657</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -2627,10 +2625,10 @@
         <v>28</v>
       </c>
       <c r="F90" s="2">
-        <v>43238.652083333327</v>
+        <v>45765.652083333327</v>
       </c>
       <c r="G90" s="2">
-        <v>43251.416666666657</v>
+        <v>45777.416666666657</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -2650,10 +2648,10 @@
         <v>28</v>
       </c>
       <c r="F91" s="2">
-        <v>43239.127083333333</v>
+        <v>45766.127083333333</v>
       </c>
       <c r="G91" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -2673,10 +2671,10 @@
         <v>28</v>
       </c>
       <c r="F92" s="2">
-        <v>43239.206250000003</v>
+        <v>45766.206250000003</v>
       </c>
       <c r="G92" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -2696,10 +2694,10 @@
         <v>30</v>
       </c>
       <c r="F93" s="2">
-        <v>43237.486805555563</v>
+        <v>45764.486805555563</v>
       </c>
       <c r="G93" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -2719,10 +2717,10 @@
         <v>30</v>
       </c>
       <c r="F94" s="2">
-        <v>43237.664583333331</v>
+        <v>45764.664583333331</v>
       </c>
       <c r="G94" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -2742,10 +2740,10 @@
         <v>30</v>
       </c>
       <c r="F95" s="2">
-        <v>43237.497916666667</v>
+        <v>45764.497916666667</v>
       </c>
       <c r="G95" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -2765,10 +2763,10 @@
         <v>30</v>
       </c>
       <c r="F96" s="2">
-        <v>43237.789583333331</v>
+        <v>45764.789583333331</v>
       </c>
       <c r="G96" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -2788,10 +2786,10 @@
         <v>30</v>
       </c>
       <c r="F97" s="2">
-        <v>43237.872916666667</v>
+        <v>45764.872916666667</v>
       </c>
       <c r="G97" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -2811,10 +2809,10 @@
         <v>30</v>
       </c>
       <c r="F98" s="2">
-        <v>43238.652083333327</v>
+        <v>45765.652083333327</v>
       </c>
       <c r="G98" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -2834,10 +2832,10 @@
         <v>30</v>
       </c>
       <c r="F99" s="2">
-        <v>43239.458333333343</v>
+        <v>45766.458333333343</v>
       </c>
       <c r="G99" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -2857,10 +2855,10 @@
         <v>30</v>
       </c>
       <c r="F100" s="2">
-        <v>43239.821527777778</v>
+        <v>45766.821527777778</v>
       </c>
       <c r="G100" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -2880,10 +2878,10 @@
         <v>30</v>
       </c>
       <c r="F101" s="2">
-        <v>43240.089583333327</v>
+        <v>45767.089583333327</v>
       </c>
       <c r="G101" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -2903,10 +2901,10 @@
         <v>32</v>
       </c>
       <c r="F102" s="2">
-        <v>43237.604166666657</v>
+        <v>45764.604166666657</v>
       </c>
       <c r="G102" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -2926,10 +2924,10 @@
         <v>32</v>
       </c>
       <c r="F103" s="2">
-        <v>43238.291666666657</v>
+        <v>45765.291666666657</v>
       </c>
       <c r="G103" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -2949,10 +2947,10 @@
         <v>32</v>
       </c>
       <c r="F104" s="2">
-        <v>43239.083333333343</v>
+        <v>45766.083333333343</v>
       </c>
       <c r="G104" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -2972,10 +2970,10 @@
         <v>32</v>
       </c>
       <c r="F105" s="2">
-        <v>43237.75</v>
+        <v>45764.75</v>
       </c>
       <c r="G105" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -2995,10 +2993,10 @@
         <v>32</v>
       </c>
       <c r="F106" s="2">
-        <v>43241.4375</v>
+        <v>45768.4375</v>
       </c>
       <c r="G106" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
@@ -3018,10 +3016,10 @@
         <v>32</v>
       </c>
       <c r="F107" s="2">
-        <v>43237.791666666657</v>
+        <v>45764.791666666657</v>
       </c>
       <c r="G107" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -3041,10 +3039,10 @@
         <v>32</v>
       </c>
       <c r="F108" s="2">
-        <v>43237.414583333331</v>
+        <v>45764.414583333331</v>
       </c>
       <c r="G108" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -3064,10 +3062,10 @@
         <v>32</v>
       </c>
       <c r="F109" s="2">
-        <v>43237.618750000001</v>
+        <v>45764.618750000001</v>
       </c>
       <c r="G109" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
@@ -3087,10 +3085,10 @@
         <v>32</v>
       </c>
       <c r="F110" s="2">
-        <v>43237.821527777778</v>
+        <v>45764.821527777778</v>
       </c>
       <c r="G110" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -3110,10 +3108,10 @@
         <v>32</v>
       </c>
       <c r="F111" s="2">
-        <v>43238.208333333343</v>
+        <v>45765.208333333343</v>
       </c>
       <c r="G111" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
@@ -3133,10 +3131,10 @@
         <v>32</v>
       </c>
       <c r="F112" s="2">
-        <v>43238.652083333327</v>
+        <v>45765.652083333327</v>
       </c>
       <c r="G112" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
@@ -3156,10 +3154,10 @@
         <v>32</v>
       </c>
       <c r="F113" s="2">
-        <v>43239.206250000003</v>
+        <v>45766.206250000003</v>
       </c>
       <c r="G113" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
@@ -3179,10 +3177,10 @@
         <v>32</v>
       </c>
       <c r="F114" s="2">
-        <v>43237.414583333331</v>
+        <v>45764.414583333331</v>
       </c>
       <c r="G114" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
@@ -3202,10 +3200,10 @@
         <v>32</v>
       </c>
       <c r="F115" s="2">
-        <v>43237.486805555563</v>
+        <v>45764.486805555563</v>
       </c>
       <c r="G115" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
@@ -3225,10 +3223,10 @@
         <v>32</v>
       </c>
       <c r="F116" s="2">
-        <v>43237.618750000001</v>
+        <v>45764.618750000001</v>
       </c>
       <c r="G116" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -3248,10 +3246,10 @@
         <v>32</v>
       </c>
       <c r="F117" s="2">
-        <v>43238.374305555553</v>
+        <v>45765.374305555553</v>
       </c>
       <c r="G117" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
@@ -3271,10 +3269,10 @@
         <v>32</v>
       </c>
       <c r="F118" s="2">
-        <v>43239.083333333343</v>
+        <v>45766.083333333343</v>
       </c>
       <c r="G118" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
@@ -3294,10 +3292,10 @@
         <v>32</v>
       </c>
       <c r="F119" s="2">
-        <v>43237.708333333343</v>
+        <v>45764.708333333343</v>
       </c>
       <c r="G119" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
@@ -3317,10 +3315,10 @@
         <v>32</v>
       </c>
       <c r="F120" s="2">
-        <v>43239.127083333333</v>
+        <v>45766.127083333333</v>
       </c>
       <c r="G120" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
@@ -3340,10 +3338,10 @@
         <v>32</v>
       </c>
       <c r="F121" s="2">
-        <v>43237.958333333343</v>
+        <v>45764.958333333343</v>
       </c>
       <c r="G121" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
@@ -3363,10 +3361,10 @@
         <v>32</v>
       </c>
       <c r="F122" s="2">
-        <v>43238.625</v>
+        <v>45765.625</v>
       </c>
       <c r="G122" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
@@ -3386,10 +3384,10 @@
         <v>32</v>
       </c>
       <c r="F123" s="2">
-        <v>43239.206250000003</v>
+        <v>45766.206250000003</v>
       </c>
       <c r="G123" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
@@ -3409,10 +3407,10 @@
         <v>32</v>
       </c>
       <c r="F124" s="2">
-        <v>43240.458333333343</v>
+        <v>45767.458333333343</v>
       </c>
       <c r="G124" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
@@ -3432,10 +3430,10 @@
         <v>32</v>
       </c>
       <c r="F125" s="2">
-        <v>43241.625</v>
+        <v>45768.625</v>
       </c>
       <c r="G125" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
@@ -3455,10 +3453,10 @@
         <v>32</v>
       </c>
       <c r="F126" s="2">
-        <v>43239.083333333343</v>
+        <v>45766.083333333343</v>
       </c>
       <c r="G126" s="2">
-        <v>43242.333333333343</v>
+        <v>45769.333333333343</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
@@ -3478,10 +3476,10 @@
         <v>32</v>
       </c>
       <c r="F127" s="2">
-        <v>43241.625</v>
+        <v>45768.625</v>
       </c>
       <c r="G127" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
@@ -3501,10 +3499,10 @@
         <v>32</v>
       </c>
       <c r="F128" s="2">
-        <v>43238.458333333343</v>
+        <v>45765.458333333343</v>
       </c>
       <c r="G128" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
@@ -3524,10 +3522,10 @@
         <v>32</v>
       </c>
       <c r="F129" s="2">
-        <v>43239.115277777782</v>
+        <v>45766.115277777782</v>
       </c>
       <c r="G129" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
@@ -3547,10 +3545,10 @@
         <v>36</v>
       </c>
       <c r="F130" s="2">
-        <v>43227.600694444453</v>
+        <v>45754.600694444453</v>
       </c>
       <c r="G130" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
@@ -3570,10 +3568,10 @@
         <v>36</v>
       </c>
       <c r="F131" s="2">
-        <v>43227.604166666657</v>
+        <v>45754.604166666657</v>
       </c>
       <c r="G131" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
@@ -3593,10 +3591,10 @@
         <v>36</v>
       </c>
       <c r="F132" s="2">
-        <v>43227.607638888891</v>
+        <v>45754.607638888891</v>
       </c>
       <c r="G132" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
@@ -3616,10 +3614,10 @@
         <v>36</v>
       </c>
       <c r="F133" s="2">
-        <v>43227.614583333343</v>
+        <v>45754.614583333343</v>
       </c>
       <c r="G133" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
@@ -3639,10 +3637,10 @@
         <v>36</v>
       </c>
       <c r="F134" s="2">
-        <v>43227.625</v>
+        <v>45754.625</v>
       </c>
       <c r="G134" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
@@ -3662,10 +3660,10 @@
         <v>36</v>
       </c>
       <c r="F135" s="2">
-        <v>43227.635416666657</v>
+        <v>45754.635416666657</v>
       </c>
       <c r="G135" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
@@ -3685,10 +3683,10 @@
         <v>36</v>
       </c>
       <c r="F136" s="2">
-        <v>43227.645833333343</v>
+        <v>45754.645833333343</v>
       </c>
       <c r="G136" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
@@ -3708,10 +3706,10 @@
         <v>36</v>
       </c>
       <c r="F137" s="2">
-        <v>43227.65625</v>
+        <v>45754.65625</v>
       </c>
       <c r="G137" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
@@ -3731,10 +3729,10 @@
         <v>36</v>
       </c>
       <c r="F138" s="2">
-        <v>43237.666666666657</v>
+        <v>45764.666666666657</v>
       </c>
       <c r="G138" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
@@ -3754,10 +3752,10 @@
         <v>36</v>
       </c>
       <c r="F139" s="2">
-        <v>43237.677083333343</v>
+        <v>45764.677083333343</v>
       </c>
       <c r="G139" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
@@ -3777,10 +3775,10 @@
         <v>36</v>
       </c>
       <c r="F140" s="2">
-        <v>43237.6875</v>
+        <v>45764.6875</v>
       </c>
       <c r="G140" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
@@ -3800,10 +3798,10 @@
         <v>36</v>
       </c>
       <c r="F141" s="2">
-        <v>43237.697916666657</v>
+        <v>45764.697916666657</v>
       </c>
       <c r="G141" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
@@ -3823,10 +3821,10 @@
         <v>36</v>
       </c>
       <c r="F142" s="2">
-        <v>43237.708333333343</v>
+        <v>45764.708333333343</v>
       </c>
       <c r="G142" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
@@ -3846,10 +3844,10 @@
         <v>36</v>
       </c>
       <c r="F143" s="2">
-        <v>43237.71875</v>
+        <v>45764.71875</v>
       </c>
       <c r="G143" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
@@ -3869,10 +3867,10 @@
         <v>36</v>
       </c>
       <c r="F144" s="2">
-        <v>43237.729166666657</v>
+        <v>45764.729166666657</v>
       </c>
       <c r="G144" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
@@ -3892,10 +3890,10 @@
         <v>36</v>
       </c>
       <c r="F145" s="2">
-        <v>43237.739583333343</v>
+        <v>45764.739583333343</v>
       </c>
       <c r="G145" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
@@ -3915,10 +3913,10 @@
         <v>36</v>
       </c>
       <c r="F146" s="2">
-        <v>43237.75</v>
+        <v>45764.75</v>
       </c>
       <c r="G146" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
@@ -3938,10 +3936,10 @@
         <v>36</v>
       </c>
       <c r="F147" s="2">
-        <v>43237.75</v>
+        <v>45764.75</v>
       </c>
       <c r="G147" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
@@ -3961,10 +3959,10 @@
         <v>36</v>
       </c>
       <c r="F148" s="2">
-        <v>43237.791666666657</v>
+        <v>45764.791666666657</v>
       </c>
       <c r="G148" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
@@ -3984,10 +3982,10 @@
         <v>36</v>
       </c>
       <c r="F149" s="2">
-        <v>43237.8125</v>
+        <v>45764.8125</v>
       </c>
       <c r="G149" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
@@ -4007,10 +4005,10 @@
         <v>36</v>
       </c>
       <c r="F150" s="2">
-        <v>43237.833333333343</v>
+        <v>45764.833333333343</v>
       </c>
       <c r="G150" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
@@ -4030,10 +4028,10 @@
         <v>36</v>
       </c>
       <c r="F151" s="2">
-        <v>43237.875</v>
+        <v>45764.875</v>
       </c>
       <c r="G151" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
@@ -4053,10 +4051,10 @@
         <v>36</v>
       </c>
       <c r="F152" s="2">
-        <v>43237.916666666657</v>
+        <v>45764.916666666657</v>
       </c>
       <c r="G152" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
@@ -4076,10 +4074,10 @@
         <v>36</v>
       </c>
       <c r="F153" s="2">
-        <v>43237.9375</v>
+        <v>45764.9375</v>
       </c>
       <c r="G153" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
@@ -4099,10 +4097,10 @@
         <v>36</v>
       </c>
       <c r="F154" s="2">
-        <v>43237.958333333343</v>
+        <v>45764.958333333343</v>
       </c>
       <c r="G154" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
@@ -4122,10 +4120,10 @@
         <v>36</v>
       </c>
       <c r="F155" s="2">
-        <v>43238</v>
+        <v>45765</v>
       </c>
       <c r="G155" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
@@ -4145,10 +4143,10 @@
         <v>36</v>
       </c>
       <c r="F156" s="2">
-        <v>43238.041666666657</v>
+        <v>45765.041666666657</v>
       </c>
       <c r="G156" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
@@ -4168,10 +4166,10 @@
         <v>36</v>
       </c>
       <c r="F157" s="2">
-        <v>43238.083333333343</v>
+        <v>45765.083333333343</v>
       </c>
       <c r="G157" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
@@ -4191,10 +4189,10 @@
         <v>36</v>
       </c>
       <c r="F158" s="2">
-        <v>43238.09375</v>
+        <v>45765.09375</v>
       </c>
       <c r="G158" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
@@ -4214,10 +4212,10 @@
         <v>36</v>
       </c>
       <c r="F159" s="2">
-        <v>43238.125</v>
+        <v>45765.125</v>
       </c>
       <c r="G159" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
@@ -4237,10 +4235,10 @@
         <v>36</v>
       </c>
       <c r="F160" s="2">
-        <v>43238.166666666657</v>
+        <v>45765.166666666657</v>
       </c>
       <c r="G160" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
@@ -4260,10 +4258,10 @@
         <v>36</v>
       </c>
       <c r="F161" s="2">
-        <v>43238.208333333343</v>
+        <v>45765.208333333343</v>
       </c>
       <c r="G161" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
@@ -4283,10 +4281,10 @@
         <v>36</v>
       </c>
       <c r="F162" s="2">
-        <v>43238.25</v>
+        <v>45765.25</v>
       </c>
       <c r="G162" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
@@ -4306,10 +4304,10 @@
         <v>36</v>
       </c>
       <c r="F163" s="2">
-        <v>43238.291666666657</v>
+        <v>45765.291666666657</v>
       </c>
       <c r="G163" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
@@ -4329,10 +4327,10 @@
         <v>36</v>
       </c>
       <c r="F164" s="2">
-        <v>43238.270833333343</v>
+        <v>45765.270833333343</v>
       </c>
       <c r="G164" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
@@ -4352,10 +4350,10 @@
         <v>36</v>
       </c>
       <c r="F165" s="2">
-        <v>43238.333333333343</v>
+        <v>45765.333333333343</v>
       </c>
       <c r="G165" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
@@ -4375,10 +4373,10 @@
         <v>36</v>
       </c>
       <c r="F166" s="2">
-        <v>43238.375</v>
+        <v>45765.375</v>
       </c>
       <c r="G166" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
@@ -4398,10 +4396,10 @@
         <v>36</v>
       </c>
       <c r="F167" s="2">
-        <v>43238.40625</v>
+        <v>45765.40625</v>
       </c>
       <c r="G167" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
@@ -4421,10 +4419,10 @@
         <v>36</v>
       </c>
       <c r="F168" s="2">
-        <v>43238.416666666657</v>
+        <v>45765.416666666657</v>
       </c>
       <c r="G168" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
@@ -4444,10 +4442,10 @@
         <v>36</v>
       </c>
       <c r="F169" s="2">
-        <v>43238.458333333343</v>
+        <v>45765.458333333343</v>
       </c>
       <c r="G169" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
@@ -4467,10 +4465,10 @@
         <v>36</v>
       </c>
       <c r="F170" s="2">
-        <v>43238.5</v>
+        <v>45765.5</v>
       </c>
       <c r="G170" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
@@ -4490,10 +4488,10 @@
         <v>36</v>
       </c>
       <c r="F171" s="2">
-        <v>43238.541666666657</v>
+        <v>45765.541666666657</v>
       </c>
       <c r="G171" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
@@ -4513,10 +4511,10 @@
         <v>36</v>
       </c>
       <c r="F172" s="2">
-        <v>43238.583333333343</v>
+        <v>45765.583333333343</v>
       </c>
       <c r="G172" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
@@ -4536,10 +4534,10 @@
         <v>36</v>
       </c>
       <c r="F173" s="2">
-        <v>43238.625</v>
+        <v>45765.625</v>
       </c>
       <c r="G173" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
@@ -4559,10 +4557,10 @@
         <v>36</v>
       </c>
       <c r="F174" s="2">
-        <v>43238.666666666657</v>
+        <v>45765.666666666657</v>
       </c>
       <c r="G174" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
@@ -4582,10 +4580,10 @@
         <v>36</v>
       </c>
       <c r="F175" s="2">
-        <v>43238.708333333343</v>
+        <v>45765.708333333343</v>
       </c>
       <c r="G175" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
@@ -4605,10 +4603,10 @@
         <v>36</v>
       </c>
       <c r="F176" s="2">
-        <v>43238.75</v>
+        <v>45765.75</v>
       </c>
       <c r="G176" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
@@ -4628,10 +4626,10 @@
         <v>36</v>
       </c>
       <c r="F177" s="2">
-        <v>43238.791666666657</v>
+        <v>45765.791666666657</v>
       </c>
       <c r="G177" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
@@ -4651,10 +4649,10 @@
         <v>36</v>
       </c>
       <c r="F178" s="2">
-        <v>43238.833333333343</v>
+        <v>45765.833333333343</v>
       </c>
       <c r="G178" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
@@ -4674,10 +4672,10 @@
         <v>36</v>
       </c>
       <c r="F179" s="2">
-        <v>43238.875</v>
+        <v>45765.875</v>
       </c>
       <c r="G179" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
@@ -4697,10 +4695,10 @@
         <v>36</v>
       </c>
       <c r="F180" s="2">
-        <v>43238.916666666657</v>
+        <v>45765.916666666657</v>
       </c>
       <c r="G180" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
@@ -4720,10 +4718,10 @@
         <v>36</v>
       </c>
       <c r="F181" s="2">
-        <v>43238.958333333343</v>
+        <v>45765.958333333343</v>
       </c>
       <c r="G181" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
@@ -4743,10 +4741,10 @@
         <v>36</v>
       </c>
       <c r="F182" s="2">
-        <v>43239</v>
+        <v>45766</v>
       </c>
       <c r="G182" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
@@ -4766,10 +4764,10 @@
         <v>36</v>
       </c>
       <c r="F183" s="2">
-        <v>43239.041666666657</v>
+        <v>45766.041666666657</v>
       </c>
       <c r="G183" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
@@ -4789,10 +4787,10 @@
         <v>36</v>
       </c>
       <c r="F184" s="2">
-        <v>43239.083333333343</v>
+        <v>45766.083333333343</v>
       </c>
       <c r="G184" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
@@ -4812,10 +4810,10 @@
         <v>36</v>
       </c>
       <c r="F185" s="2">
-        <v>43239.125</v>
+        <v>45766.125</v>
       </c>
       <c r="G185" s="2">
-        <v>43243.416666666657</v>
+        <v>45770.416666666657</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
@@ -4835,10 +4833,10 @@
         <v>36</v>
       </c>
       <c r="F186" s="2">
-        <v>43239.125</v>
+        <v>45766.125</v>
       </c>
       <c r="G186" s="2">
-        <v>43244.416666666657</v>
+        <v>45771.416666666657</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
@@ -4858,10 +4856,10 @@
         <v>36</v>
       </c>
       <c r="F187" s="2">
-        <v>43239.125</v>
+        <v>45766.125</v>
       </c>
       <c r="G187" s="2">
-        <v>43245.416666666657</v>
+        <v>45772.416666666657</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
@@ -4881,10 +4879,10 @@
         <v>36</v>
       </c>
       <c r="F188" s="2">
-        <v>43239.125</v>
+        <v>45766.125</v>
       </c>
       <c r="G188" s="2">
-        <v>43246.416666666657</v>
+        <v>45773.416666666657</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
@@ -4904,10 +4902,10 @@
         <v>36</v>
       </c>
       <c r="F189" s="2">
-        <v>43239.125</v>
+        <v>45766.125</v>
       </c>
       <c r="G189" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
@@ -4927,10 +4925,10 @@
         <v>36</v>
       </c>
       <c r="F190" s="2">
-        <v>43239.125</v>
+        <v>45766.125</v>
       </c>
       <c r="G190" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
@@ -4950,10 +4948,10 @@
         <v>36</v>
       </c>
       <c r="F191" s="2">
-        <v>43239.125</v>
+        <v>45766.125</v>
       </c>
       <c r="G191" s="2">
-        <v>43249.416666666657</v>
+        <v>45776.416666666657</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
@@ -4973,10 +4971,10 @@
         <v>36</v>
       </c>
       <c r="F192" s="2">
-        <v>43239.416666666657</v>
+        <v>45766.416666666657</v>
       </c>
       <c r="G192" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
@@ -4996,10 +4994,10 @@
         <v>36</v>
       </c>
       <c r="F193" s="2">
-        <v>43239.458333333343</v>
+        <v>45766.458333333343</v>
       </c>
       <c r="G193" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.2">
@@ -5019,10 +5017,10 @@
         <v>36</v>
       </c>
       <c r="F194" s="2">
-        <v>43239.5</v>
+        <v>45766.5</v>
       </c>
       <c r="G194" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.2">
@@ -5042,10 +5040,10 @@
         <v>36</v>
       </c>
       <c r="F195" s="2">
-        <v>43239.541666666657</v>
+        <v>45766.541666666657</v>
       </c>
       <c r="G195" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.2">
@@ -5065,10 +5063,10 @@
         <v>36</v>
       </c>
       <c r="F196" s="2">
-        <v>43239.583333333343</v>
+        <v>45766.583333333343</v>
       </c>
       <c r="G196" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.2">
@@ -5088,10 +5086,10 @@
         <v>36</v>
       </c>
       <c r="F197" s="2">
-        <v>43239.625</v>
+        <v>45766.625</v>
       </c>
       <c r="G197" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.2">
@@ -5111,10 +5109,10 @@
         <v>36</v>
       </c>
       <c r="F198" s="2">
-        <v>43239.666666666657</v>
+        <v>45766.666666666657</v>
       </c>
       <c r="G198" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.2">
@@ -5134,10 +5132,10 @@
         <v>36</v>
       </c>
       <c r="F199" s="2">
-        <v>43239.708333333343</v>
+        <v>45766.708333333343</v>
       </c>
       <c r="G199" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.2">
@@ -5157,10 +5155,10 @@
         <v>36</v>
       </c>
       <c r="F200" s="2">
-        <v>43239.75</v>
+        <v>45766.75</v>
       </c>
       <c r="G200" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
@@ -5180,10 +5178,10 @@
         <v>36</v>
       </c>
       <c r="F201" s="2">
-        <v>43239.833333333343</v>
+        <v>45766.833333333343</v>
       </c>
       <c r="G201" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
@@ -5203,10 +5201,10 @@
         <v>36</v>
       </c>
       <c r="F202" s="2">
-        <v>43239.791666666657</v>
+        <v>45766.791666666657</v>
       </c>
       <c r="G202" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
@@ -5226,10 +5224,10 @@
         <v>36</v>
       </c>
       <c r="F203" s="2">
-        <v>43239.875</v>
+        <v>45766.875</v>
       </c>
       <c r="G203" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.2">
@@ -5249,10 +5247,10 @@
         <v>36</v>
       </c>
       <c r="F204" s="2">
-        <v>43239.916666666657</v>
+        <v>45766.916666666657</v>
       </c>
       <c r="G204" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.2">
@@ -5272,10 +5270,10 @@
         <v>36</v>
       </c>
       <c r="F205" s="2">
-        <v>43239.958333333343</v>
+        <v>45766.958333333343</v>
       </c>
       <c r="G205" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
@@ -5295,10 +5293,10 @@
         <v>36</v>
       </c>
       <c r="F206" s="2">
-        <v>43240</v>
+        <v>45767</v>
       </c>
       <c r="G206" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.2">
@@ -5318,10 +5316,10 @@
         <v>36</v>
       </c>
       <c r="F207" s="2">
-        <v>43240.041666666657</v>
+        <v>45767.041666666657</v>
       </c>
       <c r="G207" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.2">
@@ -5341,10 +5339,10 @@
         <v>36</v>
       </c>
       <c r="F208" s="2">
-        <v>43240.083333333343</v>
+        <v>45767.083333333343</v>
       </c>
       <c r="G208" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.2">
@@ -5364,10 +5362,10 @@
         <v>36</v>
       </c>
       <c r="F209" s="2">
-        <v>43240.125</v>
+        <v>45767.125</v>
       </c>
       <c r="G209" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.2">
@@ -5387,10 +5385,10 @@
         <v>36</v>
       </c>
       <c r="F210" s="2">
-        <v>43240.208333333343</v>
+        <v>45767.208333333343</v>
       </c>
       <c r="G210" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.2">
@@ -5410,10 +5408,10 @@
         <v>36</v>
       </c>
       <c r="F211" s="2">
-        <v>43240.291666666657</v>
+        <v>45767.291666666657</v>
       </c>
       <c r="G211" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.2">
@@ -5433,10 +5431,10 @@
         <v>36</v>
       </c>
       <c r="F212" s="2">
-        <v>43240.375</v>
+        <v>45767.375</v>
       </c>
       <c r="G212" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.2">
@@ -5456,10 +5454,10 @@
         <v>36</v>
       </c>
       <c r="F213" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
       <c r="G213" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.2">
@@ -5479,10 +5477,10 @@
         <v>36</v>
       </c>
       <c r="F214" s="2">
-        <v>43240.458333333343</v>
+        <v>45767.458333333343</v>
       </c>
       <c r="G214" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.2">
@@ -5502,10 +5500,10 @@
         <v>36</v>
       </c>
       <c r="F215" s="2">
-        <v>43240.541666666657</v>
+        <v>45767.541666666657</v>
       </c>
       <c r="G215" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.2">
@@ -5525,10 +5523,10 @@
         <v>36</v>
       </c>
       <c r="F216" s="2">
-        <v>43240.625</v>
+        <v>45767.625</v>
       </c>
       <c r="G216" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.2">
@@ -5548,10 +5546,10 @@
         <v>36</v>
       </c>
       <c r="F217" s="2">
-        <v>43240.708333333343</v>
+        <v>45767.708333333343</v>
       </c>
       <c r="G217" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.2">
@@ -5571,10 +5569,10 @@
         <v>36</v>
       </c>
       <c r="F218" s="2">
-        <v>43240.75</v>
+        <v>45767.75</v>
       </c>
       <c r="G218" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.2">
@@ -5594,10 +5592,10 @@
         <v>36</v>
       </c>
       <c r="F219" s="2">
-        <v>43240.791666666657</v>
+        <v>45767.791666666657</v>
       </c>
       <c r="G219" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.2">
@@ -5617,10 +5615,10 @@
         <v>36</v>
       </c>
       <c r="F220" s="2">
-        <v>43240.833333333343</v>
+        <v>45767.833333333343</v>
       </c>
       <c r="G220" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.2">
@@ -5640,10 +5638,10 @@
         <v>36</v>
       </c>
       <c r="F221" s="2">
-        <v>43240.875</v>
+        <v>45767.875</v>
       </c>
       <c r="G221" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.2">
@@ -5663,10 +5661,10 @@
         <v>36</v>
       </c>
       <c r="F222" s="2">
-        <v>43240.916666666657</v>
+        <v>45767.916666666657</v>
       </c>
       <c r="G222" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.2">
@@ -5686,10 +5684,10 @@
         <v>36</v>
       </c>
       <c r="F223" s="2">
-        <v>43240.958333333343</v>
+        <v>45767.958333333343</v>
       </c>
       <c r="G223" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.2">
@@ -5709,10 +5707,10 @@
         <v>36</v>
       </c>
       <c r="F224" s="2">
-        <v>43241.041666666657</v>
+        <v>45768.041666666657</v>
       </c>
       <c r="G224" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.2">
@@ -5732,10 +5730,10 @@
         <v>36</v>
       </c>
       <c r="F225" s="2">
-        <v>43241.083333333343</v>
+        <v>45768.083333333343</v>
       </c>
       <c r="G225" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.2">
@@ -5755,10 +5753,10 @@
         <v>36</v>
       </c>
       <c r="F226" s="2">
-        <v>43241.125</v>
+        <v>45768.125</v>
       </c>
       <c r="G226" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.2">
@@ -5778,10 +5776,10 @@
         <v>36</v>
       </c>
       <c r="F227" s="2">
-        <v>43241.166666666657</v>
+        <v>45768.166666666657</v>
       </c>
       <c r="G227" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.2">
@@ -5801,10 +5799,10 @@
         <v>36</v>
       </c>
       <c r="F228" s="2">
-        <v>43241.208333333343</v>
+        <v>45768.208333333343</v>
       </c>
       <c r="G228" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.2">
@@ -5824,10 +5822,10 @@
         <v>36</v>
       </c>
       <c r="F229" s="2">
-        <v>43241.291666666657</v>
+        <v>45768.291666666657</v>
       </c>
       <c r="G229" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.2">
@@ -5847,10 +5845,10 @@
         <v>36</v>
       </c>
       <c r="F230" s="2">
-        <v>43241.333333333343</v>
+        <v>45768.333333333343</v>
       </c>
       <c r="G230" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.2">
@@ -5870,10 +5868,10 @@
         <v>36</v>
       </c>
       <c r="F231" s="2">
-        <v>43241.368055555547</v>
+        <v>45768.368055555547</v>
       </c>
       <c r="G231" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.2">
@@ -5893,10 +5891,10 @@
         <v>36</v>
       </c>
       <c r="F232" s="2">
-        <v>43241.375</v>
+        <v>45768.375</v>
       </c>
       <c r="G232" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.2">
@@ -5916,10 +5914,10 @@
         <v>36</v>
       </c>
       <c r="F233" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
       <c r="G233" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.2">
@@ -5939,10 +5937,10 @@
         <v>36</v>
       </c>
       <c r="F234" s="2">
-        <v>43241.4375</v>
+        <v>45768.4375</v>
       </c>
       <c r="G234" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.2">
@@ -5962,10 +5960,10 @@
         <v>36</v>
       </c>
       <c r="F235" s="2">
-        <v>43241.458333333343</v>
+        <v>45768.458333333343</v>
       </c>
       <c r="G235" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.2">
@@ -5985,10 +5983,10 @@
         <v>36</v>
       </c>
       <c r="F236" s="2">
-        <v>43241.46875</v>
+        <v>45768.46875</v>
       </c>
       <c r="G236" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.2">
@@ -6008,10 +6006,10 @@
         <v>36</v>
       </c>
       <c r="F237" s="2">
-        <v>43241.479166666657</v>
+        <v>45768.479166666657</v>
       </c>
       <c r="G237" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.2">
@@ -6031,10 +6029,10 @@
         <v>36</v>
       </c>
       <c r="F238" s="2">
-        <v>43241.5</v>
+        <v>45768.5</v>
       </c>
       <c r="G238" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.2">
@@ -6054,10 +6052,10 @@
         <v>36</v>
       </c>
       <c r="F239" s="2">
-        <v>43241.541666666657</v>
+        <v>45768.541666666657</v>
       </c>
       <c r="G239" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.2">
@@ -6077,10 +6075,10 @@
         <v>36</v>
       </c>
       <c r="F240" s="2">
-        <v>43241.607638888891</v>
+        <v>45768.607638888891</v>
       </c>
       <c r="G240" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.2">
@@ -6100,10 +6098,10 @@
         <v>36</v>
       </c>
       <c r="F241" s="2">
-        <v>43241.625</v>
+        <v>45768.625</v>
       </c>
       <c r="G241" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.2">
@@ -6123,10 +6121,10 @@
         <v>36</v>
       </c>
       <c r="F242" s="2">
-        <v>43241.708333333343</v>
+        <v>45768.708333333343</v>
       </c>
       <c r="G242" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.2">
@@ -6146,10 +6144,10 @@
         <v>36</v>
       </c>
       <c r="F243" s="2">
-        <v>43241.791666666657</v>
+        <v>45768.791666666657</v>
       </c>
       <c r="G243" s="2">
-        <v>43247.416666666657</v>
+        <v>45774.416666666657</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.2">
@@ -6169,10 +6167,10 @@
         <v>18</v>
       </c>
       <c r="F244" s="2">
-        <v>43237.604166666657</v>
+        <v>45764.604166666657</v>
       </c>
       <c r="G244" s="2">
-        <v>43240.416666666657</v>
+        <v>45767.416666666657</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.2">
@@ -6192,10 +6190,10 @@
         <v>18</v>
       </c>
       <c r="F245" s="2">
-        <v>43237.708333333343</v>
+        <v>45764.708333333343</v>
       </c>
       <c r="G245" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.2">
@@ -6215,10 +6213,10 @@
         <v>18</v>
       </c>
       <c r="F246" s="2">
-        <v>43237.791666666657</v>
+        <v>45764.791666666657</v>
       </c>
       <c r="G246" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.2">
@@ -6238,10 +6236,10 @@
         <v>18</v>
       </c>
       <c r="F247" s="2">
-        <v>43237.958333333343</v>
+        <v>45764.958333333343</v>
       </c>
       <c r="G247" s="2">
-        <v>43248.416666666657</v>
+        <v>45775.416666666657</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.2">
@@ -6261,10 +6259,10 @@
         <v>18</v>
       </c>
       <c r="F248" s="2">
-        <v>43238.291666666657</v>
+        <v>45765.291666666657</v>
       </c>
       <c r="G248" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.2">
@@ -6284,10 +6282,10 @@
         <v>18</v>
       </c>
       <c r="F249" s="2">
-        <v>43238.458333333343</v>
+        <v>45765.458333333343</v>
       </c>
       <c r="G249" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.2">
@@ -6307,10 +6305,10 @@
         <v>18</v>
       </c>
       <c r="F250" s="2">
-        <v>43238.625</v>
+        <v>45765.625</v>
       </c>
       <c r="G250" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.2">
@@ -6330,10 +6328,10 @@
         <v>18</v>
       </c>
       <c r="F251" s="2">
-        <v>43238.791666666657</v>
+        <v>45765.791666666657</v>
       </c>
       <c r="G251" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.2">
@@ -6353,10 +6351,10 @@
         <v>18</v>
       </c>
       <c r="F252" s="2">
-        <v>43239.083333333343</v>
+        <v>45766.083333333343</v>
       </c>
       <c r="G252" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.2">
@@ -6376,10 +6374,10 @@
         <v>18</v>
       </c>
       <c r="F253" s="2">
-        <v>43240.291666666657</v>
+        <v>45767.291666666657</v>
       </c>
       <c r="G253" s="2">
-        <v>43241.416666666657</v>
+        <v>45768.416666666657</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.2">
@@ -6399,10 +6397,10 @@
         <v>18</v>
       </c>
       <c r="F254" s="2">
-        <v>43240.458333333343</v>
+        <v>45767.458333333343</v>
       </c>
       <c r="G254" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.2">
@@ -6422,10 +6420,10 @@
         <v>18</v>
       </c>
       <c r="F255" s="2">
-        <v>43241.291666666657</v>
+        <v>45768.291666666657</v>
       </c>
       <c r="G255" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.2">
@@ -6445,10 +6443,10 @@
         <v>18</v>
       </c>
       <c r="F256" s="2">
-        <v>43241.625</v>
+        <v>45768.625</v>
       </c>
       <c r="G256" s="2">
-        <v>43242.416666666657</v>
+        <v>45769.416666666657</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.2">
@@ -6468,10 +6466,10 @@
         <v>10</v>
       </c>
       <c r="F257" s="2">
-        <v>43101</v>
+        <v>45658</v>
       </c>
       <c r="G257" s="2">
-        <v>43102</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.2">
@@ -6491,10 +6489,10 @@
         <v>10</v>
       </c>
       <c r="F258" s="2">
-        <v>43101</v>
+        <v>45658</v>
       </c>
       <c r="G258" s="2">
-        <v>43102</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.2">
@@ -6514,10 +6512,10 @@
         <v>10</v>
       </c>
       <c r="F259" s="2">
-        <v>43101</v>
+        <v>45658</v>
       </c>
       <c r="G259" s="2">
-        <v>43102</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.2">
@@ -6537,10 +6535,10 @@
         <v>10</v>
       </c>
       <c r="F260" s="2">
-        <v>43101</v>
+        <v>45658</v>
       </c>
       <c r="G260" s="2">
-        <v>43102</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.2">
@@ -6560,10 +6558,10 @@
         <v>10</v>
       </c>
       <c r="F261" s="2">
-        <v>43101</v>
+        <v>45658</v>
       </c>
       <c r="G261" s="2">
-        <v>43102</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.2">
@@ -6583,10 +6581,10 @@
         <v>10</v>
       </c>
       <c r="F262" s="2">
-        <v>43101</v>
+        <v>45658</v>
       </c>
       <c r="G262" s="2">
-        <v>43102</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.2">
@@ -6606,10 +6604,10 @@
         <v>10</v>
       </c>
       <c r="F263" s="2">
-        <v>43101</v>
+        <v>45658</v>
       </c>
       <c r="G263" s="2">
-        <v>43102</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.2">
@@ -6629,10 +6627,10 @@
         <v>10</v>
       </c>
       <c r="F264" s="2">
-        <v>43101</v>
+        <v>45658</v>
       </c>
       <c r="G264" s="2">
-        <v>43102</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.2">
@@ -6652,10 +6650,10 @@
         <v>10</v>
       </c>
       <c r="F265" s="2">
-        <v>43101</v>
+        <v>45658</v>
       </c>
       <c r="G265" s="2">
-        <v>43102</v>
+        <v>45659</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.2">
@@ -6668,14 +6666,14 @@
       <c r="C266" t="s">
         <v>25</v>
       </c>
-      <c r="D266" t="s">
-        <v>54</v>
+      <c r="D266">
+        <v>100</v>
       </c>
       <c r="E266" t="s">
         <v>26</v>
       </c>
       <c r="F266" s="2">
-        <v>43240.291666666657</v>
+        <v>45767.291666666657</v>
       </c>
       <c r="G266" s="2">
         <v>45773.012292083331</v>

</xml_diff>